<commit_message>
fix typos in profile page
</commit_message>
<xml_diff>
--- a/docs/argo-diagnosticreport.xlsx
+++ b/docs/argo-diagnosticreport.xlsx
@@ -491,10 +491,10 @@
 </t>
   </si>
   <si>
-    <t>US Core Laboratory Report Order Code</t>
-  </si>
-  <si>
-    <t>The test, panel or battery that was ordered.</t>
+    <t>US Core Report Code</t>
+  </si>
+  <si>
+    <t>The test, panel, report, or note that was ordered.</t>
   </si>
   <si>
     <t>UsageNote= The typical patterns for codes are:  1)  a LOINC code either as a  translation from a "local" code or as a primary code, or 2)  a local code only if no suitable LOINC exists,  or 3)  both the local and the LOINC translation.   Systems SHALL be capable of sending the local code if one exists.</t>
@@ -596,10 +596,10 @@
 Period {[]} {[]}</t>
   </si>
   <si>
-    <t>Time of Radiology Procedure</t>
-  </si>
-  <si>
-    <t>This is the Datetime or Period when the radiology image was done.</t>
+    <t>Time of the report or note</t>
+  </si>
+  <si>
+    <t>This is the Datetime or Period when the report or note was written.</t>
   </si>
   <si>
     <t>If the diagnostic procedure was performed on the patient, this is the time it was performed. If there are specimens, the diagnostically relevant time can be derived from the specimen collection times, but the specimen information is not always available, and the exact relationship between the specimens and the diagnostically relevant time is not always automatic.</t>

</xml_diff>